<commit_message>
Clean Up Unused Files
</commit_message>
<xml_diff>
--- a/media/template/Form Upload Excel Task.xlsx
+++ b/media/template/Form Upload Excel Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dian Putra\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58226534-6A5E-41DB-A9A2-1236FFA0B1F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E164FE9-C8DD-4803-8BD4-E46D92856AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="24240" windowHeight="12530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.5" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>